<commit_message>
Updated files, corrected 2.5 yr variable
</commit_message>
<xml_diff>
--- a/Data/Commongarden.xlsx
+++ b/Data/Commongarden.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\livvel\Documents\Callunachildren\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92704F57-4967-4C94-AED8-9CAEE9DA7022}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D643EAA6-6322-4458-A88F-3EFCDA6DB720}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{E0723129-6D22-4097-926A-005274B47CB9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{E0723129-6D22-4097-926A-005274B47CB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Commongarden" sheetId="1" r:id="rId1"/>
@@ -560,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8AC26CB-AFBC-4127-A966-1CD438524518}">
-  <dimension ref="A1:Q2161"/>
+  <dimension ref="A1:P2161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" topLeftCell="A317" workbookViewId="0">
+      <selection activeCell="O360" sqref="O360"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2043,10 +2043,10 @@
         <v>1</v>
       </c>
       <c r="O48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>1</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>1</v>
       </c>
@@ -2080,7 +2080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>1</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>1</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>1</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>1</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>1</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>1</v>
       </c>
@@ -2209,11 +2209,11 @@
       <c r="O56">
         <v>1</v>
       </c>
-      <c r="Q56" t="s">
+      <c r="P56" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>1</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>1</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>1</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>1</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>1</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>1</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>1</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>1</v>
       </c>
@@ -3855,7 +3855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>1</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>1</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>1</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>1</v>
       </c>
@@ -4013,7 +4013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>1</v>
       </c>
@@ -4057,11 +4057,11 @@
       <c r="O117">
         <v>0</v>
       </c>
-      <c r="Q117" t="s">
+      <c r="P117" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>1</v>
       </c>
@@ -4108,7 +4108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>1</v>
       </c>
@@ -4155,7 +4155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>1</v>
       </c>
@@ -4202,7 +4202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>1</v>
       </c>
@@ -4249,7 +4249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>2</v>
       </c>
@@ -4296,7 +4296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>2</v>
       </c>
@@ -4313,7 +4313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>2</v>
       </c>
@@ -4360,7 +4360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>2</v>
       </c>
@@ -4377,7 +4377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>2</v>
       </c>
@@ -4394,7 +4394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>2</v>
       </c>
@@ -4441,7 +4441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>2</v>
       </c>
@@ -45854,7 +45854,7 @@
         <v>31</v>
       </c>
       <c r="C1542" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D1542">
         <v>3834</v>
@@ -45901,7 +45901,7 @@
         <v>31</v>
       </c>
       <c r="C1543" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="D1543">
         <v>2249</v>
@@ -45918,7 +45918,7 @@
         <v>31</v>
       </c>
       <c r="C1544" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D1544">
         <v>1306</v>
@@ -47277,7 +47277,7 @@
         <v>36</v>
       </c>
       <c r="D1592">
-        <v>3846</v>
+        <v>2846</v>
       </c>
       <c r="O1592">
         <v>1</v>

</xml_diff>